<commit_message>
Fixed update data access and filtered already added roles api call
</commit_message>
<xml_diff>
--- a/data/roles/UserRoleAssignment 7.xlsx
+++ b/data/roles/UserRoleAssignment 7.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation NEW\Roles-DataAccess\data\roles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AATools\Roles-DataAccess\data\roles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>INIT_IN_HYDERABAD</t>
+  </si>
+  <si>
+    <t>ADD</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,6 +1283,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
@@ -1291,7 +1305,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added code for create users
</commit_message>
<xml_diff>
--- a/data/roles/UserRoleAssignment 7.xlsx
+++ b/data/roles/UserRoleAssignment 7.xlsx
@@ -12,11 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Roles" sheetId="1" r:id="rId1"/>
-    <sheet name="DataAccess" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId1"/>
+    <sheet name="Roles" sheetId="1" r:id="rId2"/>
+    <sheet name="DataAccess" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DataAccess!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataAccess!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -48,9 +49,6 @@
     <t>Operation</t>
   </si>
   <si>
-    <t>Raj</t>
-  </si>
-  <si>
     <t>Manufacturing Engineer</t>
   </si>
   <si>
@@ -67,13 +65,43 @@
   </si>
   <si>
     <t>ADD</t>
+  </si>
+  <si>
+    <t>Ramesh.Arvapalli</t>
+  </si>
+  <si>
+    <t>USER_NAME</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>user@test.com</t>
+  </si>
+  <si>
+    <t>test_user2</t>
+  </si>
+  <si>
+    <t>REMOVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +116,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF707070"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,12 +150,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1259,10 +1294,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,13 +1369,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1300,12 +1395,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,51 +1425,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed minor bugs for report not refreshing
</commit_message>
<xml_diff>
--- a/data/roles/UserRoleAssignment 7.xlsx
+++ b/data/roles/UserRoleAssignment 7.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="3" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="DataAccess" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataAccess!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DataAccess!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -49,25 +49,7 @@
     <t>Operation</t>
   </si>
   <si>
-    <t>Manufacturing Engineer</t>
-  </si>
-  <si>
-    <t>Manufacturing plant</t>
-  </si>
-  <si>
-    <t>INIT_US_SPRING</t>
-  </si>
-  <si>
-    <t>INIT_NL_AMSTERDAM</t>
-  </si>
-  <si>
-    <t>INIT_IN_HYDERABAD</t>
-  </si>
-  <si>
     <t>ADD</t>
-  </si>
-  <si>
-    <t>Ramesh.Arvapalli</t>
   </si>
   <si>
     <t>USER_NAME</t>
@@ -82,19 +64,22 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Kerry</t>
+    <t>AA_LEASE_ROLE</t>
   </si>
   <si>
-    <t>Jones</t>
+    <t>INIT US BU</t>
   </si>
   <si>
-    <t>user@test.com</t>
+    <t>Business unit</t>
   </si>
   <si>
-    <t>test_user2</t>
+    <t>a</t>
   </si>
   <si>
-    <t>REMOVE</t>
+    <t>rama</t>
+  </si>
+  <si>
+    <t>ramesharvapa101@appsassociates.com</t>
   </si>
 </sst>
 </file>
@@ -118,10 +103,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF707070"/>
-      <name val="Segoe UI"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,18 +134,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1297,61 +1286,65 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -1368,47 +1361,333 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
+      <c r="A2" s="4" t="s">
+        <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,51 +1704,731 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="5"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="5"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="5"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="5"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="5"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="5"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="5"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="5"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="5"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="5"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="5"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="5"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="5"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="5"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="5"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="5"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="5"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="5"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="5"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="5"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="5"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="5"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="5"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="5"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="5"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="5"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="5"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="5"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="5"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="5"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="5"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="5"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="5"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="5"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="5"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="5"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="5"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="5"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="5"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="5"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="5"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="5"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="5"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="5"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="5"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="5"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="5"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="5"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="5"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="5"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="5"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="5"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="5"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="5"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="5"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="5"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="5"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="5"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="5"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="5"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="5"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="5"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="5"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="5"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="5"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="5"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="5"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="5"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="5"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="5"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="5"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="5"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="5"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="5"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="5"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="5"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="5"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>